<commit_message>
Update Gurobi and cplex options
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/FragilityCurvesData/ProbabilityEachScenario.xlsx
+++ b/CreateBaseDeck/FragilityCurvesData/ProbabilityEachScenario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,34 +525,6 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>2045</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.8099999999999999</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>2050</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.8099999999999999</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.04</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>